<commit_message>
examples updated for v17.01
</commit_message>
<xml_diff>
--- a/Examples/Data/Documents/Excel.xlsx
+++ b/Examples/Data/Documents/Excel.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,9 +14,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>hail hydra</t>
+  </si>
+  <si>
+    <t>pause</t>
+  </si>
+  <si>
+    <t>structure</t>
+  </si>
+  <si>
+    <t>paws</t>
+  </si>
+  <si>
+    <t>pores</t>
+  </si>
+  <si>
+    <t>pours</t>
+  </si>
+  <si>
+    <t>braze</t>
   </si>
 </sst>
 </file>
@@ -114,7 +132,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -149,7 +167,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -358,9 +376,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -369,6 +389,36 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
examples updated for version 17.03
</commit_message>
<xml_diff>
--- a/Examples/Data/Documents/Excel.xlsx
+++ b/Examples/Data/Documents/Excel.xlsx
@@ -376,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,6 +419,21 @@
         <v>6</v>
       </c>
     </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>